<commit_message>
Minor features and Configurations
</commit_message>
<xml_diff>
--- a/output/RIFT_V2/dump/test.xlsx
+++ b/output/RIFT_V2/dump/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64931733c3934785/Documents/Q4 2022/Fishing Tournament 2021 Repos/dump/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64931733c3934785/Documents/Q4 2022/Proyecto de Graduacion Fase I/Fishing Tournament 2021 Repos/gui/src/dump/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_46DD91AB5F82495A5AB01DFFAC26882B4E6F449B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78C6B63B-526A-4AB5-99F4-CCA22A6F27B9}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_C397A48590C49F65A0009B91FC9F206BB3F9F560" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3ACA983-692D-452D-BA7A-70DA6FD57F64}"/>
   <bookViews>
-    <workbookView xWindow="20565" yWindow="3360" windowWidth="14970" windowHeight="15345" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2670" yWindow="2985" windowWidth="14970" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inscription" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,24 @@
     <sheet name="Kids" sheetId="5" r:id="rId5"/>
     <sheet name="Women" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -57,26 +69,121 @@
     <t>WOMEN_PRESENT</t>
   </si>
   <si>
-    <t>Bote</t>
-  </si>
-  <si>
-    <t>Prueba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(123) 456-7890
-</t>
-  </si>
-  <si>
-    <t>marzo651@gmail.com</t>
+    <t>PARTICIPATION FEE</t>
+  </si>
+  <si>
+    <t>TOTAL FEES</t>
+  </si>
+  <si>
+    <t>Titanic</t>
+  </si>
+  <si>
+    <t>Robin Arellano</t>
+  </si>
+  <si>
+    <t>(102)555 5555</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
   </si>
   <si>
     <t>Participating</t>
+  </si>
+  <si>
+    <t>Olimpic</t>
+  </si>
+  <si>
+    <t>Bobby Schwalter</t>
+  </si>
+  <si>
+    <t>Costic</t>
+  </si>
+  <si>
+    <t>Genghis Khan</t>
+  </si>
+  <si>
+    <t>Costa Concordia</t>
+  </si>
+  <si>
+    <t>Reventuki Reventar</t>
+  </si>
+  <si>
+    <t>Not Participating</t>
+  </si>
+  <si>
+    <t>Titanica</t>
+  </si>
+  <si>
+    <t>Genghis Khans</t>
+  </si>
+  <si>
+    <t>(555)100 5555</t>
+  </si>
+  <si>
+    <t>email@test.com</t>
+  </si>
+  <si>
+    <t>HOOKUP_ID</t>
+  </si>
+  <si>
+    <t>HOOKUP_TIME</t>
+  </si>
+  <si>
+    <t>FISH</t>
+  </si>
+  <si>
+    <t>RELEASE_TIME</t>
+  </si>
+  <si>
+    <t>CLEAN_RELEASE</t>
+  </si>
+  <si>
+    <t>POINTS</t>
+  </si>
+  <si>
+    <t>18:08:39</t>
+  </si>
+  <si>
+    <t>Blue Marlin</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>18:13:14</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>19:33:15</t>
+  </si>
+  <si>
+    <t>Dolphin</t>
+  </si>
+  <si>
+    <t>22:46:48</t>
+  </si>
+  <si>
+    <t>18:13:44</t>
+  </si>
+  <si>
+    <t>Barracuda</t>
+  </si>
+  <si>
+    <t>18:14:25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,8 +213,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,27 +518,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,37 +571,195 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <f>IF(F2="Participating",700,0)+IF(G2="Participating",350,0)+IF(H2="Participating",300,0)+IF(I2="Participating",50,0)+IF(J2="Participating",50,0)</f>
+        <v>1450</v>
+      </c>
+      <c r="N2" s="1">
+        <f>SUM(K:K)</f>
+        <v>6550</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <f>IF(F3="Participating",700,0)+IF(G3="Participating",350,0)+IF(H3="Participating",300,0)+IF(I3="Participating",50,0)+IF(J3="Participating",50,0)</f>
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <f>IF(F4="Participating",700,0)+IF(G4="Participating",350,0)+IF(H4="Participating",300,0)+IF(I4="Participating",50,0)+IF(J4="Participating",50,0)</f>
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5">
+        <f>VALUE(IF(F5="Participating",700,0)+IF(G5="Participating",350,0)+IF(H5="Participating",300,0)+IF(I5="Participating",50,0)+IF(J5="Participating",50,0))</f>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6">
+        <f>IF(F6="Participating",700,0)+IF(G6="Participating",350,0)+IF(H6="Participating",300,0)+IF(I6="Participating",50,0)+IF(J6="Participating",50,0)</f>
+        <v>1450</v>
       </c>
     </row>
   </sheetData>
@@ -501,6 +769,298 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7">
+        <v>550</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -511,40 +1071,102 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>